<commit_message>
Removed the hardcoded password and omported it as an environment vairiable. Then i ran the code today on 15-Aug-2025
</commit_message>
<xml_diff>
--- a/INVESTMENT  - 24-Apr-2025.xlsx
+++ b/INVESTMENT  - 24-Apr-2025.xlsx
@@ -1193,7 +1193,7 @@
         <v>2648.28</v>
       </c>
       <c r="I2" s="67" t="n">
-        <v>3144.2</v>
+        <v>3265.4</v>
       </c>
       <c r="J2" s="48">
         <f>G2*H2</f>
@@ -1297,7 +1297,7 @@
         <v>2381.91</v>
       </c>
       <c r="I3" s="67" t="n">
-        <v>1971.9</v>
+        <v>1936.6</v>
       </c>
       <c r="J3" s="48">
         <f>G3*H3</f>
@@ -1399,7 +1399,7 @@
         <v>81.28</v>
       </c>
       <c r="I4" s="54" t="n">
-        <v>89.81</v>
+        <v>90.5</v>
       </c>
       <c r="J4" s="55">
         <f>G4*H4</f>
@@ -1500,7 +1500,7 @@
         <v>157.16</v>
       </c>
       <c r="I5" s="54" t="n">
-        <v>166.9</v>
+        <v>168.06</v>
       </c>
       <c r="J5" s="55">
         <f>G5*H5</f>
@@ -1601,7 +1601,7 @@
         <v>19.8</v>
       </c>
       <c r="I6" s="54" t="n">
-        <v>21.51</v>
+        <v>21.69</v>
       </c>
       <c r="J6" s="55">
         <f>G6*H6</f>
@@ -1682,7 +1682,7 @@
       </c>
       <c r="D7" s="95" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>B_N_Y</t>
         </is>
       </c>
       <c r="E7" s="95" t="inlineStr">
@@ -1702,7 +1702,7 @@
         <v>22.22</v>
       </c>
       <c r="I7" s="54" t="n">
-        <v>24.1</v>
+        <v>24.76</v>
       </c>
       <c r="J7" s="55">
         <f>G7*H7</f>
@@ -1783,7 +1783,7 @@
       </c>
       <c r="D8" s="95" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>B_N_Y</t>
         </is>
       </c>
       <c r="E8" s="95" t="inlineStr">
@@ -1803,7 +1803,7 @@
         <v>58.09</v>
       </c>
       <c r="I8" s="54" t="n">
-        <v>58.55</v>
+        <v>58.35</v>
       </c>
       <c r="J8" s="55">
         <f>G8*H8</f>
@@ -1903,7 +1903,7 @@
         <v>68.84999999999999</v>
       </c>
       <c r="I9" s="60" t="n">
-        <v>87.19</v>
+        <v>85.95</v>
       </c>
       <c r="J9" s="59">
         <f>G9*H9</f>
@@ -1983,7 +1983,7 @@
       </c>
       <c r="D10" s="95" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>B_N_Y</t>
         </is>
       </c>
       <c r="E10" s="95" t="inlineStr">
@@ -2003,7 +2003,7 @@
         <v>142.45</v>
       </c>
       <c r="I10" s="54" t="n">
-        <v>144.85</v>
+        <v>150.22</v>
       </c>
       <c r="J10" s="55">
         <f>G10*H10</f>
@@ -2104,7 +2104,7 @@
         <v>95.88</v>
       </c>
       <c r="I11" s="60" t="n">
-        <v>115.64</v>
+        <v>115.33</v>
       </c>
       <c r="J11" s="59">
         <f>G11*H11</f>
@@ -2196,7 +2196,7 @@
         <v>55.53</v>
       </c>
       <c r="I12" s="74" t="n">
-        <v>85.01000000000001</v>
+        <v>83.8</v>
       </c>
       <c r="J12" s="69">
         <f>G12*H12</f>
@@ -2296,7 +2296,7 @@
         <v>50.15</v>
       </c>
       <c r="I13" s="70" t="n">
-        <v>47.86</v>
+        <v>48.23</v>
       </c>
       <c r="J13" s="68">
         <f>G13*H13</f>
@@ -2400,7 +2400,7 @@
         <v>180.73</v>
       </c>
       <c r="I14" s="54" t="n">
-        <v>202.09</v>
+        <v>204.89</v>
       </c>
       <c r="J14" s="55">
         <f>G14*H14</f>
@@ -2493,7 +2493,7 @@
         <v>75.68000000000001</v>
       </c>
       <c r="I15" s="74" t="n">
-        <v>110.97</v>
+        <v>110.83</v>
       </c>
       <c r="J15" s="69">
         <f>G15*H15</f>
@@ -2589,7 +2589,7 @@
         <v>418.8</v>
       </c>
       <c r="I16" s="54" t="n">
-        <v>375.08</v>
+        <v>379.83</v>
       </c>
       <c r="J16" s="55">
         <f>G16*H16</f>
@@ -2690,7 +2690,7 @@
         <v>26.36</v>
       </c>
       <c r="I17" s="54" t="n">
-        <v>29.4</v>
+        <v>29.82</v>
       </c>
       <c r="J17" s="55">
         <f>G17*H17</f>
@@ -2791,7 +2791,7 @@
         <v>514.8200000000001</v>
       </c>
       <c r="I18" s="54" t="n">
-        <v>563.02</v>
+        <v>567</v>
       </c>
       <c r="J18" s="55">
         <f>G18*H18</f>
@@ -2862,7 +2862,7 @@
       </c>
       <c r="D19" s="95" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>S</t>
         </is>
       </c>
       <c r="E19" s="95" t="inlineStr">
@@ -2882,7 +2882,7 @@
         <v>256.53</v>
       </c>
       <c r="I19" s="60" t="n">
-        <v>259.98</v>
+        <v>263.12</v>
       </c>
       <c r="J19" s="59">
         <f>G19*H19</f>
@@ -3434,7 +3434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CI17"/>
+  <dimension ref="A1:CJ17"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="BJ1" activePane="topRight" state="frozen"/>
@@ -3891,6 +3891,11 @@
           <t>2025-08-10 17:48</t>
         </is>
       </c>
+      <c r="CJ1" t="inlineStr">
+        <is>
+          <t>2025-08-15 20:05</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="28.8" customHeight="1">
       <c r="A2" s="46" t="inlineStr">
@@ -4038,6 +4043,11 @@
           <t>B_N_Y</t>
         </is>
       </c>
+      <c r="CJ2" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="46" t="inlineStr">
@@ -4470,6 +4480,11 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CJ3" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="52" t="inlineStr">
@@ -4902,6 +4917,11 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CJ4" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="52" t="inlineStr">
@@ -5334,6 +5354,11 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CJ5" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="52" t="inlineStr">
@@ -5766,6 +5791,11 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CJ6" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="52" t="inlineStr">
@@ -6198,6 +6228,11 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CJ7" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="52" t="inlineStr">
@@ -6630,6 +6665,11 @@
           <t>B</t>
         </is>
       </c>
+      <c r="CJ8" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="18" customHeight="1">
       <c r="A9" s="59" t="inlineStr">
@@ -7062,6 +7102,11 @@
           <t>B_N_Y</t>
         </is>
       </c>
+      <c r="CJ9" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="52" t="inlineStr">
@@ -7494,6 +7539,11 @@
           <t>B</t>
         </is>
       </c>
+      <c r="CJ10" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="18" customHeight="1">
       <c r="A11" s="59" t="inlineStr">
@@ -7926,6 +7976,11 @@
           <t>B</t>
         </is>
       </c>
+      <c r="CJ11" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="68" t="inlineStr">
@@ -8358,6 +8413,11 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CJ12" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="52" t="inlineStr">
@@ -8790,6 +8850,11 @@
           <t>B_N_Y</t>
         </is>
       </c>
+      <c r="CJ13" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="52" t="inlineStr">
@@ -9222,6 +9287,11 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CJ14" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="52" t="inlineStr">
@@ -9654,6 +9724,11 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CJ15" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="52" t="inlineStr">
@@ -10086,6 +10161,11 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CJ16" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="17" ht="18" customHeight="1">
       <c r="A17" s="59" t="inlineStr">
@@ -10516,6 +10596,11 @@
       <c r="CI17" t="inlineStr">
         <is>
           <t>B</t>
+        </is>
+      </c>
+      <c r="CJ17" t="inlineStr">
+        <is>
+          <t>S</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Run on 18-Aug-2025. Converted teh datetime object to Date entry for the table
</commit_message>
<xml_diff>
--- a/INVESTMENT  - 24-Apr-2025.xlsx
+++ b/INVESTMENT  - 24-Apr-2025.xlsx
@@ -1193,7 +1193,7 @@
         <v>2648.28</v>
       </c>
       <c r="I2" s="67" t="n">
-        <v>3265.4</v>
+        <v>3416.4</v>
       </c>
       <c r="J2" s="48">
         <f>G2*H2</f>
@@ -1297,7 +1297,7 @@
         <v>2381.91</v>
       </c>
       <c r="I3" s="67" t="n">
-        <v>1936.6</v>
+        <v>2005.6</v>
       </c>
       <c r="J3" s="48">
         <f>G3*H3</f>
@@ -1399,7 +1399,7 @@
         <v>81.28</v>
       </c>
       <c r="I4" s="54" t="n">
-        <v>90.5</v>
+        <v>90.75</v>
       </c>
       <c r="J4" s="55">
         <f>G4*H4</f>
@@ -1500,7 +1500,7 @@
         <v>157.16</v>
       </c>
       <c r="I5" s="54" t="n">
-        <v>168.06</v>
+        <v>169.94</v>
       </c>
       <c r="J5" s="55">
         <f>G5*H5</f>
@@ -1601,7 +1601,7 @@
         <v>19.8</v>
       </c>
       <c r="I6" s="54" t="n">
-        <v>21.69</v>
+        <v>21.95</v>
       </c>
       <c r="J6" s="55">
         <f>G6*H6</f>
@@ -1702,7 +1702,7 @@
         <v>22.22</v>
       </c>
       <c r="I7" s="54" t="n">
-        <v>24.76</v>
+        <v>25.88</v>
       </c>
       <c r="J7" s="55">
         <f>G7*H7</f>
@@ -1803,7 +1803,7 @@
         <v>58.09</v>
       </c>
       <c r="I8" s="54" t="n">
-        <v>58.35</v>
+        <v>59.47</v>
       </c>
       <c r="J8" s="55">
         <f>G8*H8</f>
@@ -1903,7 +1903,7 @@
         <v>68.84999999999999</v>
       </c>
       <c r="I9" s="60" t="n">
-        <v>85.95</v>
+        <v>85.67</v>
       </c>
       <c r="J9" s="59">
         <f>G9*H9</f>
@@ -2003,7 +2003,7 @@
         <v>142.45</v>
       </c>
       <c r="I10" s="54" t="n">
-        <v>150.22</v>
+        <v>149.66</v>
       </c>
       <c r="J10" s="55">
         <f>G10*H10</f>
@@ -2104,7 +2104,7 @@
         <v>95.88</v>
       </c>
       <c r="I11" s="60" t="n">
-        <v>115.33</v>
+        <v>114.35</v>
       </c>
       <c r="J11" s="59">
         <f>G11*H11</f>
@@ -2196,7 +2196,7 @@
         <v>55.53</v>
       </c>
       <c r="I12" s="74" t="n">
-        <v>83.8</v>
+        <v>83.56999999999999</v>
       </c>
       <c r="J12" s="69">
         <f>G12*H12</f>
@@ -2296,7 +2296,7 @@
         <v>50.15</v>
       </c>
       <c r="I13" s="70" t="n">
-        <v>48.23</v>
+        <v>48.87</v>
       </c>
       <c r="J13" s="68">
         <f>G13*H13</f>
@@ -2400,7 +2400,7 @@
         <v>180.73</v>
       </c>
       <c r="I14" s="54" t="n">
-        <v>204.89</v>
+        <v>205.79</v>
       </c>
       <c r="J14" s="55">
         <f>G14*H14</f>
@@ -2493,7 +2493,7 @@
         <v>75.68000000000001</v>
       </c>
       <c r="I15" s="74" t="n">
-        <v>110.83</v>
+        <v>109.87</v>
       </c>
       <c r="J15" s="69">
         <f>G15*H15</f>
@@ -2589,7 +2589,7 @@
         <v>418.8</v>
       </c>
       <c r="I16" s="54" t="n">
-        <v>379.83</v>
+        <v>378.29</v>
       </c>
       <c r="J16" s="55">
         <f>G16*H16</f>
@@ -2670,7 +2670,7 @@
       </c>
       <c r="D17" s="95" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>B_N_Y</t>
         </is>
       </c>
       <c r="E17" s="95" t="inlineStr">
@@ -2690,7 +2690,7 @@
         <v>26.36</v>
       </c>
       <c r="I17" s="54" t="n">
-        <v>29.82</v>
+        <v>30.42</v>
       </c>
       <c r="J17" s="55">
         <f>G17*H17</f>
@@ -2791,7 +2791,7 @@
         <v>514.8200000000001</v>
       </c>
       <c r="I18" s="54" t="n">
-        <v>567</v>
+        <v>571.23</v>
       </c>
       <c r="J18" s="55">
         <f>G18*H18</f>
@@ -2882,7 +2882,7 @@
         <v>256.53</v>
       </c>
       <c r="I19" s="60" t="n">
-        <v>263.12</v>
+        <v>266</v>
       </c>
       <c r="J19" s="59">
         <f>G19*H19</f>
@@ -3434,7 +3434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CJ17"/>
+  <dimension ref="A1:CL17"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="BJ1" activePane="topRight" state="frozen"/>
@@ -3896,6 +3896,16 @@
           <t>2025-08-15 20:05</t>
         </is>
       </c>
+      <c r="CK1" t="inlineStr">
+        <is>
+          <t>2025-08-18 09:44</t>
+        </is>
+      </c>
+      <c r="CL1" t="inlineStr">
+        <is>
+          <t>2025-08-18 10:18</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="28.8" customHeight="1">
       <c r="A2" s="46" t="inlineStr">
@@ -4048,6 +4058,16 @@
           <t>B_N_Y</t>
         </is>
       </c>
+      <c r="CK2" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
+      <c r="CL2" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="46" t="inlineStr">
@@ -4485,6 +4505,16 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CK3" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="CL3" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="52" t="inlineStr">
@@ -4922,6 +4952,16 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CK4" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="CL4" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="52" t="inlineStr">
@@ -5359,6 +5399,16 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CK5" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="CL5" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="52" t="inlineStr">
@@ -5796,6 +5846,16 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CK6" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="CL6" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="52" t="inlineStr">
@@ -6233,6 +6293,16 @@
           <t>B_N_Y</t>
         </is>
       </c>
+      <c r="CK7" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
+      <c r="CL7" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="52" t="inlineStr">
@@ -6670,6 +6740,16 @@
           <t>B_N_Y</t>
         </is>
       </c>
+      <c r="CK8" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
+      <c r="CL8" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="18" customHeight="1">
       <c r="A9" s="59" t="inlineStr">
@@ -7107,6 +7187,16 @@
           <t>B_N_Y</t>
         </is>
       </c>
+      <c r="CK9" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
+      <c r="CL9" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="52" t="inlineStr">
@@ -7544,6 +7634,16 @@
           <t>B_N_Y</t>
         </is>
       </c>
+      <c r="CK10" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
+      <c r="CL10" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="18" customHeight="1">
       <c r="A11" s="59" t="inlineStr">
@@ -7981,6 +8081,16 @@
           <t>B</t>
         </is>
       </c>
+      <c r="CK11" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="CL11" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="68" t="inlineStr">
@@ -8418,6 +8528,16 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CK12" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="CL12" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="52" t="inlineStr">
@@ -8855,6 +8975,16 @@
           <t>B_N_Y</t>
         </is>
       </c>
+      <c r="CK13" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
+      <c r="CL13" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="52" t="inlineStr">
@@ -9292,6 +9422,16 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CK14" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="CL14" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="52" t="inlineStr">
@@ -9729,6 +9869,16 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CK15" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
+      <c r="CL15" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="52" t="inlineStr">
@@ -10166,6 +10316,16 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CK16" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="CL16" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="17" ht="18" customHeight="1">
       <c r="A17" s="59" t="inlineStr">
@@ -10599,6 +10759,16 @@
         </is>
       </c>
       <c r="CJ17" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="CK17" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="CL17" t="inlineStr">
         <is>
           <t>S</t>
         </is>

</xml_diff>

<commit_message>
28-Aug-2025 Run. Now saving the data of the TA Analysis after adding all th erelevt columns with EMA and RSI details of each individual stocks.
</commit_message>
<xml_diff>
--- a/INVESTMENT  - 24-Apr-2025.xlsx
+++ b/INVESTMENT  - 24-Apr-2025.xlsx
@@ -1193,7 +1193,7 @@
         <v>2648.28</v>
       </c>
       <c r="I2" s="67" t="n">
-        <v>3354</v>
+        <v>3395.6</v>
       </c>
       <c r="J2" s="48">
         <f>G2*H2</f>
@@ -1297,7 +1297,7 @@
         <v>2381.91</v>
       </c>
       <c r="I3" s="67" t="n">
-        <v>2010</v>
+        <v>2041.8</v>
       </c>
       <c r="J3" s="48">
         <f>G3*H3</f>
@@ -1399,7 +1399,7 @@
         <v>81.28</v>
       </c>
       <c r="I4" s="54" t="n">
-        <v>90.31</v>
+        <v>90.34</v>
       </c>
       <c r="J4" s="55">
         <f>G4*H4</f>
@@ -1500,7 +1500,7 @@
         <v>157.16</v>
       </c>
       <c r="I5" s="54" t="n">
-        <v>171.43</v>
+        <v>171.77</v>
       </c>
       <c r="J5" s="55">
         <f>G5*H5</f>
@@ -1601,7 +1601,7 @@
         <v>19.8</v>
       </c>
       <c r="I6" s="54" t="n">
-        <v>22.14</v>
+        <v>22.24</v>
       </c>
       <c r="J6" s="55">
         <f>G6*H6</f>
@@ -1702,7 +1702,7 @@
         <v>22.22</v>
       </c>
       <c r="I7" s="54" t="n">
-        <v>26.12</v>
+        <v>26.11</v>
       </c>
       <c r="J7" s="55">
         <f>G7*H7</f>
@@ -1803,7 +1803,7 @@
         <v>58.09</v>
       </c>
       <c r="I8" s="54" t="n">
-        <v>59.7</v>
+        <v>60.35</v>
       </c>
       <c r="J8" s="55">
         <f>G8*H8</f>
@@ -1903,7 +1903,7 @@
         <v>68.84999999999999</v>
       </c>
       <c r="I9" s="60" t="n">
-        <v>85</v>
+        <v>84.77</v>
       </c>
       <c r="J9" s="59">
         <f>G9*H9</f>
@@ -2003,7 +2003,7 @@
         <v>142.45</v>
       </c>
       <c r="I10" s="54" t="n">
-        <v>150.11</v>
+        <v>148.98</v>
       </c>
       <c r="J10" s="55">
         <f>G10*H10</f>
@@ -2104,7 +2104,7 @@
         <v>95.88</v>
       </c>
       <c r="I11" s="60" t="n">
-        <v>113.96</v>
+        <v>111.44</v>
       </c>
       <c r="J11" s="59">
         <f>G11*H11</f>
@@ -2196,7 +2196,7 @@
         <v>55.53</v>
       </c>
       <c r="I12" s="74" t="n">
-        <v>82.84999999999999</v>
+        <v>82.69</v>
       </c>
       <c r="J12" s="69">
         <f>G12*H12</f>
@@ -2296,7 +2296,7 @@
         <v>50.15</v>
       </c>
       <c r="I13" s="70" t="n">
-        <v>49.44</v>
+        <v>49.67</v>
       </c>
       <c r="J13" s="68">
         <f>G13*H13</f>
@@ -2400,7 +2400,7 @@
         <v>180.73</v>
       </c>
       <c r="I14" s="54" t="n">
-        <v>205.48</v>
+        <v>203.48</v>
       </c>
       <c r="J14" s="55">
         <f>G14*H14</f>
@@ -2493,7 +2493,7 @@
         <v>75.68000000000001</v>
       </c>
       <c r="I15" s="74" t="n">
-        <v>109.41</v>
+        <v>106.99</v>
       </c>
       <c r="J15" s="69">
         <f>G15*H15</f>
@@ -2589,7 +2589,7 @@
         <v>418.8</v>
       </c>
       <c r="I16" s="54" t="n">
-        <v>378.88</v>
+        <v>388.71</v>
       </c>
       <c r="J16" s="55">
         <f>G16*H16</f>
@@ -2690,7 +2690,7 @@
         <v>26.36</v>
       </c>
       <c r="I17" s="54" t="n">
-        <v>30.44</v>
+        <v>30.3</v>
       </c>
       <c r="J17" s="55">
         <f>G17*H17</f>
@@ -2791,7 +2791,7 @@
         <v>514.8200000000001</v>
       </c>
       <c r="I18" s="54" t="n">
-        <v>572.36</v>
+        <v>570.8</v>
       </c>
       <c r="J18" s="55">
         <f>G18*H18</f>
@@ -2882,7 +2882,7 @@
         <v>263.37</v>
       </c>
       <c r="I19" s="60" t="n">
-        <v>266.48</v>
+        <v>267.07</v>
       </c>
       <c r="J19" s="59">
         <f>G19*H19</f>
@@ -3434,7 +3434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CO17"/>
+  <dimension ref="A1:CQ17"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="BJ1" activePane="topRight" state="frozen"/>
@@ -3921,6 +3921,16 @@
           <t>2025-08-19 23:51</t>
         </is>
       </c>
+      <c r="CP1" t="inlineStr">
+        <is>
+          <t>2025-08-20 16:14</t>
+        </is>
+      </c>
+      <c r="CQ1" t="inlineStr">
+        <is>
+          <t>2025-08-20 16:19</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="28.8" customHeight="1">
       <c r="A2" s="46" t="inlineStr">
@@ -4098,6 +4108,16 @@
           <t>B_N_Y</t>
         </is>
       </c>
+      <c r="CP2" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
+      <c r="CQ2" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="46" t="inlineStr">
@@ -4560,6 +4580,16 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CP3" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="CQ3" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="52" t="inlineStr">
@@ -5022,6 +5052,16 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CP4" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="CQ4" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="52" t="inlineStr">
@@ -5484,6 +5524,16 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CP5" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="CQ5" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="52" t="inlineStr">
@@ -5946,6 +5996,16 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CP6" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="CQ6" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="52" t="inlineStr">
@@ -6408,6 +6468,16 @@
           <t>B_N_Y</t>
         </is>
       </c>
+      <c r="CP7" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
+      <c r="CQ7" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="52" t="inlineStr">
@@ -6870,6 +6940,16 @@
           <t>B_N_Y</t>
         </is>
       </c>
+      <c r="CP8" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
+      <c r="CQ8" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="18" customHeight="1">
       <c r="A9" s="59" t="inlineStr">
@@ -7332,6 +7412,16 @@
           <t>B_N_Y</t>
         </is>
       </c>
+      <c r="CP9" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
+      <c r="CQ9" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="52" t="inlineStr">
@@ -7794,6 +7884,16 @@
           <t>B_N_Y</t>
         </is>
       </c>
+      <c r="CP10" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
+      <c r="CQ10" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="18" customHeight="1">
       <c r="A11" s="59" t="inlineStr">
@@ -8256,6 +8356,16 @@
           <t>B</t>
         </is>
       </c>
+      <c r="CP11" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="CQ11" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="68" t="inlineStr">
@@ -8718,6 +8828,16 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CP12" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="CQ12" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="52" t="inlineStr">
@@ -9180,6 +9300,16 @@
           <t>B_N_Y</t>
         </is>
       </c>
+      <c r="CP13" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
+      <c r="CQ13" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="52" t="inlineStr">
@@ -9642,6 +9772,16 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CP14" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="CQ14" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="52" t="inlineStr">
@@ -10104,6 +10244,16 @@
           <t>B_N_Y</t>
         </is>
       </c>
+      <c r="CP15" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
+      <c r="CQ15" t="inlineStr">
+        <is>
+          <t>B_N_Y</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="52" t="inlineStr">
@@ -10566,6 +10716,16 @@
           <t>S</t>
         </is>
       </c>
+      <c r="CP16" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="CQ16" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
     </row>
     <row r="17" ht="18" customHeight="1">
       <c r="A17" s="59" t="inlineStr">
@@ -11024,6 +11184,16 @@
         </is>
       </c>
       <c r="CO17" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="CP17" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="CQ17" t="inlineStr">
         <is>
           <t>B</t>
         </is>

</xml_diff>